<commit_message>
Updated for latest algo of calcs for stitch determiner
</commit_message>
<xml_diff>
--- a/charts_xlsx/kschart.xlsx
+++ b/charts_xlsx/kschart.xlsx
@@ -928,12 +928,11 @@
     <t xml:space="preserve">211: [-5 APPLYING TRINE to MOON; 7 APPLYING OPPOSITION to VENUS; -2 SEPARATING SQUARE to JUPITER; 2 SEPARATING SQUARE to SATURN] </t>
   </si>
   <si>
-    <t>211: [STITCH DETERMINER FOR: APPLYING TRINE (ASC, MOON) [Score:Intensity: TRINE:8, Exactness:-5, Collective Planet Speed:10] 
+    <t>211: [STITCH DETERMINER FOR: APPLYING TRINE (ASC, MOON) [Score:Intensity: TRINE:8 - Exactness:-5, Calc Score:3] 
 Diamonds, Triangles, or Leaves 
- Exactness Stitch Width: 5 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [10, 0] 
- Tot Dig Score: 1]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Planet Scores: 0, 11 
+ Orb Width: 8]</t>
   </si>
   <si>
     <t>213</t>
@@ -1197,12 +1196,11 @@
     <t xml:space="preserve">326: [-5 APPLYING TRINE to ASC; 2 SEPARATING SEXTILE to VENUS; 7 SEPARATING TRINE to MARS; -2 APPLYING SEMISQUARE to URANUS; 6 SEPARATING SQUARE to PLUTO] </t>
   </si>
   <si>
-    <t>326: [STITCH DETERMINER FOR: APPLYING TRINE (MOON, ASC) [Score:Intensity: TRINE:8, Exactness:-5, Collective Planet Speed:10] 
+    <t>326: [STITCH DETERMINER FOR: APPLYING TRINE (MOON, ASC) [Score:Intensity: TRINE:8 - Exactness:-5, Calc Score:3] 
 Diamonds, Triangles, or Leaves 
- Exactness Stitch Width: 5 
  Aspect K/P:PatternStitchBase.KNIT 
- Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Speed Stitch Width: [10, 0] 
- Tot Dig Score: 1]</t>
+ Planets K/P: [&lt;PatternStitchBase.KNIT: 1&gt;, &lt;PatternStitchBase.KNIT: 1&gt;] Planet Scores: 11, 0 
+ Orb Width: 8]</t>
   </si>
   <si>
     <t>327</t>

</xml_diff>